<commit_message>
Planilha Reforma Tributária v3
</commit_message>
<xml_diff>
--- a/Extensão-InvoiCy-Sheets/ModeloPlanilha_Emissao_Reforma_tributaria.xlsx
+++ b/Extensão-InvoiCy-Sheets/ModeloPlanilha_Emissao_Reforma_tributaria.xlsx
@@ -912,8 +912,8 @@
   </sheetPr>
   <dimension ref="A1:EN1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DZ1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="DZ3" activeCellId="0" sqref="DZ3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1007,7 +1007,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="142" min="142" style="1" width="20.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="143" min="143" style="1" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="144" min="144" style="1" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1446,7 +1446,7 @@
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>144</v>

</xml_diff>

<commit_message>
Novos campos no Grupo AtividadeEvento
</commit_message>
<xml_diff>
--- a/Extensão-InvoiCy-Sheets/ModeloPlanilha_Emissao_Reforma_tributaria.xlsx
+++ b/Extensão-InvoiCy-Sheets/ModeloPlanilha_Emissao_Reforma_tributaria.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="208">
   <si>
     <t xml:space="preserve">versaoPlanilha</t>
   </si>
@@ -457,6 +457,42 @@
     <t xml:space="preserve">CodigoNBS</t>
   </si>
   <si>
+    <t xml:space="preserve">AtivDesc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivDataInicial</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivDataFinal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivIdEvento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivEndLogradouro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivEndNumero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivEndCompl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivEndBairro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivEndCEP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivEndcMun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivEndxMun</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AtivEndUF</t>
+  </si>
+  <si>
     <t xml:space="preserve">RPS</t>
   </si>
   <si>
@@ -590,6 +626,24 @@
   </si>
   <si>
     <t xml:space="preserve">Reembolso de despesas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atividade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logradouro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complemento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bairro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SP</t>
   </si>
 </sst>
 </file>
@@ -636,16 +690,15 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Liberation Mono;Courier New;Dej"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Liberation Mono;Courier New;DejaVu Sans Mono;Lucida Sans Typewriter"/>
-      <family val="3"/>
-      <charset val="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -696,7 +749,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -717,7 +770,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -733,11 +786,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -924,10 +981,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:EO1000"/>
+  <dimension ref="A1:FA1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="DY1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="EO2" activeCellId="0" sqref="EO2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="ES3" activeCellId="0" sqref="ES3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -935,56 +992,56 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="20.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="6.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="9.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="6.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="12.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="14.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="9.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="9.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="6.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="1" width="9.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="1" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="1" width="11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="27" style="1" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="8.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="10.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="1" width="8.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="1" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="1" width="11.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="5.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="10.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="8.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="1" width="5.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="1" width="10.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="1" width="8.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="1" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="1" width="11.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="11.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="5.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="1" width="11.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="1" width="5.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="1" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="19.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="32.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="1" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="43" min="43" style="1" width="32.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="1" width="8.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="45" style="1" width="14.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="1" width="9.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="1" width="7.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="19.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="1" width="19.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="1" width="14.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="1" width="14.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="1" width="19.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="54" style="1" width="14.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="19.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="1" width="19.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="1" width="42.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="61" min="61" style="1" width="15.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="1" width="19.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="1" width="15.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="1" width="15.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="1" width="20.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="1" width="16.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="71" min="71" style="1" width="17.71"/>
@@ -993,11 +1050,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="74" min="74" style="1" width="15.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="85" min="85" style="1" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="86" min="86" style="1" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="1" width="13.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="87" min="87" style="1" width="13.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="89" min="88" style="1" width="14.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="91" min="91" style="1" width="15.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="92" min="92" style="1" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="1" width="12.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="93" min="93" style="1" width="12.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="94" min="94" style="1" width="16.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="99" min="98" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="100" min="100" style="1" width="14.14"/>
@@ -1005,23 +1062,24 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="103" min="103" style="1" width="17.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="106" min="106" style="1" width="13.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="108" min="107" style="1" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="112" min="112" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="112" min="112" style="1" width="15.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="116" min="116" style="1" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="119" min="119" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="122" min="122" style="1" width="25.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="127" min="127" style="1" width="15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="128" min="128" style="1" width="16.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="130" min="129" style="1" width="20.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="133" min="133" style="1" width="35.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="1" width="15.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="133" min="133" style="1" width="35.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="134" min="134" style="1" width="15.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="138" min="138" style="1" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="139" min="139" style="1" width="15.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="140" min="140" style="1" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="141" min="141" style="1" width="15.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="142" min="142" style="1" width="20.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="142" min="142" style="1" width="20.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="143" min="143" style="1" width="18.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="144" min="144" style="1" width="44.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="145" min="145" style="1" width="16.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="148" min="147" style="0" width="20.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
@@ -1461,13 +1519,49 @@
       <c r="EO1" s="5" t="s">
         <v>144</v>
       </c>
+      <c r="EP1" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="EQ1" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="ER1" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="ES1" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="ET1" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="EU1" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="EV1" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="EW1" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="EX1" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="EY1" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="EZ1" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="FA1" s="5" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>100</v>
@@ -1497,79 +1591,79 @@
         <v>2</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="P2" s="2" t="n">
         <v>2</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="T2" s="7" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="Z2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AA2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AB2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AC2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AG2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AH2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AI2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AJ2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="AL2" s="2" t="n">
         <v>3</v>
@@ -1587,7 +1681,7 @@
         <v>1234</v>
       </c>
       <c r="AQ2" s="2" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
       <c r="AR2" s="2" t="n">
         <v>3550308</v>
@@ -1599,28 +1693,28 @@
         <v>99999999000191</v>
       </c>
       <c r="AW2" s="2" t="s">
-        <v>152</v>
+        <v>164</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>153</v>
+        <v>165</v>
       </c>
       <c r="AY2" s="2" t="s">
-        <v>154</v>
+        <v>166</v>
       </c>
       <c r="AZ2" s="2" t="n">
         <v>3000</v>
       </c>
       <c r="BA2" s="2" t="s">
-        <v>155</v>
+        <v>167</v>
       </c>
       <c r="BB2" s="2" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="BC2" s="2" t="n">
         <v>3550308</v>
       </c>
       <c r="BD2" s="2" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="BE2" s="2" t="n">
         <v>98700000</v>
@@ -1629,10 +1723,10 @@
         <v>5535354800</v>
       </c>
       <c r="BG2" s="2" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="BH2" s="2" t="s">
-        <v>159</v>
+        <v>171</v>
       </c>
       <c r="BI2" s="1" t="n">
         <v>4321808</v>
@@ -1653,118 +1747,118 @@
         <v>3</v>
       </c>
       <c r="BO2" s="9" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="BP2" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="BQ2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="BR2" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="BS2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="BT2" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="BU2" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="BV2" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="BW2" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="BX2" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="BY2" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="BZ2" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="CA2" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="CB2" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="BQ2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="BR2" s="9" t="s">
-        <v>147</v>
-      </c>
-      <c r="BS2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="BT2" s="9" t="s">
+      <c r="CC2" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="BU2" s="9" t="s">
-        <v>163</v>
-      </c>
-      <c r="BV2" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="BW2" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="BX2" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="BY2" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="BZ2" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="CA2" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="CB2" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="CC2" s="9" t="s">
-        <v>150</v>
-      </c>
       <c r="CD2" s="9" t="s">
-        <v>168</v>
+        <v>180</v>
       </c>
       <c r="CE2" s="9" t="s">
-        <v>169</v>
+        <v>181</v>
       </c>
       <c r="CF2" s="9" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="CG2" s="9" t="s">
-        <v>170</v>
+        <v>182</v>
       </c>
       <c r="CH2" s="9" t="s">
-        <v>171</v>
+        <v>183</v>
       </c>
       <c r="CI2" s="9" t="s">
-        <v>172</v>
+        <v>184</v>
       </c>
       <c r="CJ2" s="9" t="s">
-        <v>161</v>
+        <v>173</v>
       </c>
       <c r="CK2" s="9" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="CL2" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="CM2" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="CN2" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="CO2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="CP2" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="CQ2" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="CR2" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="CS2" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="CT2" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="CM2" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="CN2" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="CO2" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="CP2" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="CQ2" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="CR2" s="9" t="s">
-        <v>164</v>
-      </c>
-      <c r="CS2" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="CT2" s="9" t="s">
-        <v>161</v>
-      </c>
       <c r="CU2" s="9" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="CV2" s="9" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="CW2" s="9" t="s">
-        <v>175</v>
+        <v>187</v>
       </c>
       <c r="CX2" s="9" t="s">
-        <v>176</v>
+        <v>188</v>
       </c>
       <c r="CY2" s="9" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="CZ2" s="9" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="DA2" s="9" t="n">
         <v>220</v>
@@ -1776,7 +1870,7 @@
         <v>3550308</v>
       </c>
       <c r="DD2" s="9" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="DE2" s="9" t="n">
         <v>101</v>
@@ -1794,37 +1888,37 @@
         <v>40558577456</v>
       </c>
       <c r="DJ2" s="9" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
       <c r="DK2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="DL2" s="9" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="DM2" s="9" t="s">
-        <v>180</v>
+        <v>192</v>
       </c>
       <c r="DN2" s="9" t="n">
         <v>1000</v>
       </c>
       <c r="DO2" s="9" t="s">
-        <v>181</v>
+        <v>193</v>
       </c>
       <c r="DP2" s="9" t="s">
-        <v>182</v>
+        <v>194</v>
       </c>
       <c r="DQ2" s="9" t="n">
         <v>11987654321</v>
       </c>
       <c r="DR2" s="9" t="s">
-        <v>183</v>
+        <v>195</v>
       </c>
       <c r="DS2" s="9" t="n">
         <v>3550308</v>
       </c>
       <c r="DT2" s="9" t="s">
-        <v>177</v>
+        <v>189</v>
       </c>
       <c r="DU2" s="9" t="n">
         <v>1311000</v>
@@ -1833,16 +1927,16 @@
         <v>1058</v>
       </c>
       <c r="DW2" s="9" t="s">
-        <v>184</v>
+        <v>196</v>
       </c>
       <c r="DX2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="DY2" s="9" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="DZ2" s="9" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="EA2" s="9" t="n">
         <v>3550308</v>
@@ -1851,7 +1945,7 @@
         <v>25352</v>
       </c>
       <c r="EC2" s="9" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="ED2" s="9" t="n">
         <v>45682010000104</v>
@@ -1860,13 +1954,13 @@
         <v>40558488521</v>
       </c>
       <c r="EF2" s="9" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="EG2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="EH2" s="9" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="EI2" s="9" t="n">
         <v>45658</v>
@@ -1878,16 +1972,52 @@
         <v>1</v>
       </c>
       <c r="EL2" s="9" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="EM2" s="9" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="EN2" s="9" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="EO2" s="10" t="n">
         <v>101011100</v>
+      </c>
+      <c r="EP2" s="0" t="s">
+        <v>202</v>
+      </c>
+      <c r="EQ2" s="6" t="n">
+        <v>44387.3333333333</v>
+      </c>
+      <c r="ER2" s="6" t="n">
+        <v>44387.3333333333</v>
+      </c>
+      <c r="ES2" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="ET2" s="0" t="s">
+        <v>204</v>
+      </c>
+      <c r="EU2" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="EV2" s="0" t="s">
+        <v>205</v>
+      </c>
+      <c r="EW2" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="EX2" s="0" t="n">
+        <v>18240000</v>
+      </c>
+      <c r="EY2" s="11" t="n">
+        <v>3550308</v>
+      </c>
+      <c r="EZ2" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="FA2" s="0" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>